<commit_message>
Made the time plan a lot more friendly :)
</commit_message>
<xml_diff>
--- a/doc/Time-Plan.xlsx
+++ b/doc/Time-Plan.xlsx
@@ -16,95 +16,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>Democratic Conferencing Tool</t>
   </si>
   <si>
-    <t>Prototype</t>
-  </si>
-  <si>
     <t>Robert</t>
   </si>
   <si>
-    <t>Specification</t>
-  </si>
-  <si>
-    <t>Implementation</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
     <t>Henry</t>
   </si>
   <si>
-    <t>Evaluation</t>
-  </si>
-  <si>
     <t>Tammie</t>
   </si>
   <si>
-    <t>Interim report</t>
-  </si>
-  <si>
     <t>William</t>
   </si>
   <si>
-    <t>Updated and expanded description of the problem to be solved</t>
-  </si>
-  <si>
-    <t>Background information and research</t>
-  </si>
-  <si>
-    <t>Requirements specification for the system to be built</t>
-  </si>
-  <si>
-    <t>Initial design of the proposed system and its user interface</t>
-  </si>
-  <si>
-    <t>Record of key implementation decisions</t>
-  </si>
-  <si>
-    <t>Results of any initial implementation steps/prototyping</t>
-  </si>
-  <si>
-    <t>Discussion of any problems encountered so far</t>
-  </si>
-  <si>
     <t>Group</t>
   </si>
   <si>
-    <t>Time plan for the project</t>
-  </si>
-  <si>
-    <t>Final System</t>
-  </si>
-  <si>
     <t>Henry,Carl</t>
   </si>
   <si>
-    <t>Final Group Report</t>
-  </si>
-  <si>
-    <t>Updated design of the system and its user interface</t>
-  </si>
-  <si>
-    <t>Discussion on the implementation and testing of the system</t>
-  </si>
-  <si>
-    <t>Summary of what was achieved</t>
-  </si>
-  <si>
-    <t>Reflective comments on the success of the project</t>
-  </si>
-  <si>
-    <t>An appendix giving a description of how the developed system was tested</t>
-  </si>
-  <si>
-    <t>Minutes from all formal meetings</t>
-  </si>
-  <si>
     <t>Duration (Days)</t>
   </si>
   <si>
@@ -142,6 +76,69 @@
   </si>
   <si>
     <t>Henry, Carl</t>
+  </si>
+  <si>
+    <t>Prototype Specification</t>
+  </si>
+  <si>
+    <t>Prototype Implementation</t>
+  </si>
+  <si>
+    <t>Prototype Testing</t>
+  </si>
+  <si>
+    <t>Prototype Evaluation</t>
+  </si>
+  <si>
+    <t>Interim Report: The Problem</t>
+  </si>
+  <si>
+    <t>Interim Report: Background research</t>
+  </si>
+  <si>
+    <t>Interim Report:  Requirements spec.</t>
+  </si>
+  <si>
+    <t>Interim Report: Initial design</t>
+  </si>
+  <si>
+    <t>Interim Report: Key implementation decisions</t>
+  </si>
+  <si>
+    <t>Interim Report: Problems encountered so far</t>
+  </si>
+  <si>
+    <t>Interim Report: Time plan</t>
+  </si>
+  <si>
+    <t>Final System: Implementation</t>
+  </si>
+  <si>
+    <t>Final System: Testing</t>
+  </si>
+  <si>
+    <t>Final Report: Updated designs</t>
+  </si>
+  <si>
+    <t>Final Report: Discussion on implementation/testing</t>
+  </si>
+  <si>
+    <t>Final Report: Summary of what was achieved</t>
+  </si>
+  <si>
+    <t>Final Report: Reflective comments</t>
+  </si>
+  <si>
+    <t>Final Report: Appendix with testing</t>
+  </si>
+  <si>
+    <t>Interim Report: Initial implementation/prototyping</t>
+  </si>
+  <si>
+    <t>Final Report: Appendix with minutes</t>
+  </si>
+  <si>
+    <t>Interim Report</t>
   </si>
 </sst>
 </file>
@@ -197,6 +194,427 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Start Date</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="25"/>
+                <c:pt idx="1">
+                  <c:v>Prototype Specification</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Prototype Implementation</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Prototype Testing</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Prototype Evaluation</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Interim Report</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Interim Report: The Problem</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Interim Report: Background research</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Interim Report:  Requirements spec.</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Interim Report: Initial design</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Interim Report: Key implementation decisions</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Interim Report: Initial implementation/prototyping</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Interim Report: Problems encountered so far</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Interim Report: Time plan</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Final System: Implementation</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Final System: Testing</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Final Report: Updated designs</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Final Report: Discussion on implementation/testing</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Final Report: Summary of what was achieved</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Final Report: Reflective comments</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Final Report: Appendix with testing</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Final Report: Appendix with minutes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>d/m/yyyy</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="1">
+                  <c:v>40126</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40135</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40135</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40126</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40145</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40126</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40129</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40129</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40129</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40129</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40138</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40126</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40148</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40168</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40154</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40161</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40224</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40224</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40168</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40224</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Duration (Days)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="25"/>
+                <c:pt idx="1">
+                  <c:v>Prototype Specification</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Prototype Implementation</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Prototype Testing</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Prototype Evaluation</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Interim Report</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Interim Report: The Problem</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Interim Report: Background research</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Interim Report:  Requirements spec.</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Interim Report: Initial design</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Interim Report: Key implementation decisions</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Interim Report: Initial implementation/prototyping</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Interim Report: Problems encountered so far</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Interim Report: Time plan</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Final System: Implementation</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Final System: Testing</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Final Report: Updated designs</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Final Report: Discussion on implementation/testing</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Final Report: Summary of what was achieved</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Final Report: Reflective comments</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Final Report: Appendix with testing</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Final Report: Appendix with minutes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:overlap val="100"/>
+        <c:axId val="47591424"/>
+        <c:axId val="70533504"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="47591424"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="70533504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="70533504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="40126"/>
+        </c:scaling>
+        <c:axPos val="t"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="d/m/yyyy" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9525"/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" baseline="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="47591424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>526677</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>168089</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>89647</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>123264</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -486,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -500,19 +918,19 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -532,27 +950,14 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3">
-        <v>40126</v>
-      </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3">
-        <f t="shared" ref="D3:D27" si="0">B3+C3</f>
-        <v>40136</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="D3" s="3"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>40126</v>
@@ -561,17 +966,17 @@
         <v>2</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D4:D27" si="0">B4+C4</f>
         <v>40128</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B5" s="3">
         <v>40128</v>
@@ -584,232 +989,216 @@
         <v>40135</v>
       </c>
       <c r="E5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3">
-        <v>40137</v>
+        <v>40135</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" si="0"/>
         <v>40138</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3">
-        <v>40137</v>
+        <v>40135</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" si="0"/>
         <v>40138</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3">
-        <v>40126</v>
-      </c>
-      <c r="C8">
-        <v>20</v>
-      </c>
-      <c r="D8" s="3">
-        <f t="shared" si="0"/>
-        <v>40146</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="D8" s="3"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>11</v>
+      <c r="A9" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="B9" s="3">
         <v>40126</v>
       </c>
       <c r="C9">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" si="0"/>
-        <v>40146</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
+        <v>40152</v>
       </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3">
-        <v>40126</v>
+        <v>40145</v>
       </c>
       <c r="C10">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" si="0"/>
-        <v>40146</v>
+        <v>40151</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B11" s="3">
         <v>40126</v>
       </c>
       <c r="C11">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" si="0"/>
-        <v>40146</v>
+        <v>40131</v>
       </c>
       <c r="E11" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B12" s="3">
-        <v>40126</v>
+        <v>40129</v>
       </c>
       <c r="C12">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>40146</v>
+        <v>40134</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B13" s="3">
-        <v>40126</v>
+        <v>40129</v>
       </c>
       <c r="C13">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="0"/>
-        <v>40146</v>
+        <v>40134</v>
       </c>
       <c r="E13" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B14" s="3">
-        <v>40126</v>
+        <v>40129</v>
       </c>
       <c r="C14">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="0"/>
-        <v>40146</v>
+        <v>40138</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B15" s="3">
-        <v>40126</v>
+        <v>40129</v>
       </c>
       <c r="C15">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D15" s="3">
         <f t="shared" si="0"/>
-        <v>40146</v>
+        <v>40141</v>
       </c>
       <c r="E15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B16" s="3">
+        <v>40138</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>40145</v>
+      </c>
+      <c r="E16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="3">
         <v>40126</v>
       </c>
-      <c r="C16">
-        <v>20</v>
-      </c>
-      <c r="D16" s="3">
-        <f t="shared" si="0"/>
-        <v>40146</v>
-      </c>
-      <c r="E16" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="3">
-        <v>40140</v>
-      </c>
       <c r="C17">
-        <v>94</v>
+        <v>5</v>
       </c>
       <c r="D17" s="3">
         <f t="shared" si="0"/>
-        <v>40234</v>
+        <v>40131</v>
       </c>
       <c r="E17" t="s">
         <v>2</v>
@@ -817,198 +1206,173 @@
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="3">
-        <v>40140</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-      <c r="D18" s="3">
-        <f t="shared" si="0"/>
-        <v>40143</v>
-      </c>
-      <c r="E18" t="s">
-        <v>34</v>
-      </c>
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="D18" s="3"/>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B19" s="3">
-        <v>40143</v>
+        <v>40148</v>
       </c>
       <c r="C19">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="D19" s="3">
         <f t="shared" si="0"/>
-        <v>40211</v>
+        <v>40235</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B20" s="3">
-        <v>40224</v>
+        <v>40168</v>
       </c>
       <c r="C20">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="D20" s="3">
         <f t="shared" si="0"/>
-        <v>40240</v>
+        <v>40242</v>
       </c>
       <c r="E20" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="3">
-        <v>40154</v>
-      </c>
-      <c r="C21">
-        <v>84</v>
-      </c>
-      <c r="D21" s="3">
-        <f t="shared" si="0"/>
-        <v>40238</v>
-      </c>
-      <c r="E21" t="s">
-        <v>10</v>
-      </c>
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="D21" s="3"/>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B22" s="3">
         <v>40154</v>
       </c>
       <c r="C22">
-        <v>84</v>
+        <v>28</v>
       </c>
       <c r="D22" s="3">
         <f t="shared" si="0"/>
-        <v>40238</v>
+        <v>40182</v>
       </c>
       <c r="E22" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B23" s="3">
-        <v>40154</v>
+        <v>40161</v>
       </c>
       <c r="C23">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="D23" s="3">
         <f t="shared" si="0"/>
-        <v>40238</v>
+        <v>40182</v>
       </c>
       <c r="E23" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B24" s="3">
-        <v>40154</v>
+        <v>40224</v>
       </c>
       <c r="C24">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="D24" s="3">
         <f t="shared" si="0"/>
-        <v>40238</v>
+        <v>40245</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B25" s="3">
-        <v>40154</v>
+        <v>40224</v>
       </c>
       <c r="C25">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="D25" s="3">
         <f t="shared" si="0"/>
-        <v>40238</v>
+        <v>40245</v>
       </c>
       <c r="E25" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B26" s="3">
-        <v>40154</v>
+        <v>40168</v>
       </c>
       <c r="C26">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D26" s="3">
         <f t="shared" si="0"/>
-        <v>40238</v>
+        <v>40242</v>
       </c>
       <c r="E26" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B27" s="3">
-        <v>40154</v>
+        <v>40224</v>
       </c>
       <c r="C27">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="D27" s="3">
         <f t="shared" si="0"/>
         <v>40238</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Modified timeplan - changed problems encountered to Tammy
</commit_message>
<xml_diff>
--- a/doc/Time-Plan.xlsx
+++ b/doc/Time-Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>Democratic Conferencing Tool</t>
   </si>
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>William</t>
-  </si>
-  <si>
-    <t>Group</t>
   </si>
   <si>
     <t>Henry,Carl</t>
@@ -528,24 +525,24 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="47591424"/>
-        <c:axId val="70533504"/>
+        <c:axId val="68859392"/>
+        <c:axId val="68860928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="47591424"/>
+        <c:axId val="68859392"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70533504"/>
+        <c:crossAx val="68860928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70533504"/>
+        <c:axId val="68860928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="40126"/>
@@ -567,7 +564,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47591424"/>
+        <c:crossAx val="68859392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -576,7 +573,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -904,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -918,19 +915,19 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -957,7 +954,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="3">
         <v>40126</v>
@@ -970,13 +967,13 @@
         <v>40128</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3">
         <v>40128</v>
@@ -995,7 +992,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="3">
         <v>40135</v>
@@ -1014,7 +1011,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="3">
         <v>40135</v>
@@ -1039,7 +1036,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" s="3">
         <v>40126</v>
@@ -1055,7 +1052,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3">
         <v>40145</v>
@@ -1074,7 +1071,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="3">
         <v>40126</v>
@@ -1087,13 +1084,13 @@
         <v>40131</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="3">
         <v>40129</v>
@@ -1112,7 +1109,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="3">
         <v>40129</v>
@@ -1125,13 +1122,13 @@
         <v>40134</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="3">
         <v>40129</v>
@@ -1150,7 +1147,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="3">
         <v>40129</v>
@@ -1163,13 +1160,13 @@
         <v>40141</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="3">
         <v>40138</v>
@@ -1182,13 +1179,13 @@
         <v>40145</v>
       </c>
       <c r="E16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="3">
         <v>40126</v>
@@ -1213,7 +1210,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="3">
         <v>40148</v>
@@ -1226,13 +1223,13 @@
         <v>40235</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="3">
         <v>40168</v>
@@ -1245,7 +1242,7 @@
         <v>40242</v>
       </c>
       <c r="E20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -1257,7 +1254,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" s="3">
         <v>40154</v>
@@ -1270,13 +1267,13 @@
         <v>40182</v>
       </c>
       <c r="E22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="3">
         <v>40161</v>
@@ -1289,13 +1286,13 @@
         <v>40182</v>
       </c>
       <c r="E23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" s="3">
         <v>40224</v>
@@ -1308,13 +1305,13 @@
         <v>40245</v>
       </c>
       <c r="E24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25" s="3">
         <v>40224</v>
@@ -1333,7 +1330,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="3">
         <v>40168</v>
@@ -1346,13 +1343,13 @@
         <v>40242</v>
       </c>
       <c r="E26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" s="3">
         <v>40224</v>

</xml_diff>

<commit_message>
Making changes at home - Billy
</commit_message>
<xml_diff>
--- a/doc/Time-Plan.xlsx
+++ b/doc/Time-Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
   <si>
     <t>Democratic Conferencing Tool</t>
   </si>
@@ -30,12 +30,6 @@
     <t>Tammie</t>
   </si>
   <si>
-    <t>William</t>
-  </si>
-  <si>
-    <t>Henry,Carl</t>
-  </si>
-  <si>
     <t>Duration (Days)</t>
   </si>
   <si>
@@ -57,24 +51,12 @@
     <t>Carl, Kit</t>
   </si>
   <si>
-    <t>William, Robert, Tammie, Carl</t>
-  </si>
-  <si>
-    <t>Robert, William</t>
-  </si>
-  <si>
     <t>Tammie, Robert</t>
   </si>
   <si>
-    <t>Robert, Henry, Carl</t>
-  </si>
-  <si>
     <t>Robert, Billy</t>
   </si>
   <si>
-    <t>Henry, Carl</t>
-  </si>
-  <si>
     <t>Prototype Specification</t>
   </si>
   <si>
@@ -93,9 +75,6 @@
     <t>Interim Report: Background research</t>
   </si>
   <si>
-    <t>Interim Report:  Requirements spec.</t>
-  </si>
-  <si>
     <t>Interim Report: Initial design</t>
   </si>
   <si>
@@ -108,18 +87,9 @@
     <t>Interim Report: Time plan</t>
   </si>
   <si>
-    <t>Final System: Implementation</t>
-  </si>
-  <si>
     <t>Final System: Testing</t>
   </si>
   <si>
-    <t>Final Report: Updated designs</t>
-  </si>
-  <si>
-    <t>Final Report: Discussion on implementation/testing</t>
-  </si>
-  <si>
     <t>Final Report: Summary of what was achieved</t>
   </si>
   <si>
@@ -136,13 +106,91 @@
   </si>
   <si>
     <t>Interim Report</t>
+  </si>
+  <si>
+    <t>Final Report</t>
+  </si>
+  <si>
+    <t>Billy, Robert, Tammie, Carl</t>
+  </si>
+  <si>
+    <t>Billy</t>
+  </si>
+  <si>
+    <t>Robert, Billy, Henry, Carl, Kit, Tammie</t>
+  </si>
+  <si>
+    <t>Final System</t>
+  </si>
+  <si>
+    <t>Robert, Tammie, Henry, Carl</t>
+  </si>
+  <si>
+    <t>Prototyping</t>
+  </si>
+  <si>
+    <t>Robert, Kit, Tammie, Henry</t>
+  </si>
+  <si>
+    <t>Final System: Template Coding</t>
+  </si>
+  <si>
+    <t>Final System: Interface Design</t>
+  </si>
+  <si>
+    <t>Tammie, Carl</t>
+  </si>
+  <si>
+    <t>Final Report: Introduction</t>
+  </si>
+  <si>
+    <t>Billy, Henry</t>
+  </si>
+  <si>
+    <t>Billy, Tammie</t>
+  </si>
+  <si>
+    <t>Billy, Robert, Henry, Carl</t>
+  </si>
+  <si>
+    <t>Final Report: Additional research</t>
+  </si>
+  <si>
+    <t>Billy, Robert</t>
+  </si>
+  <si>
+    <t>Final Report: Condensed existing research</t>
+  </si>
+  <si>
+    <t>Final Report: Discussion on implementation of software</t>
+  </si>
+  <si>
+    <t>Interim Report: Requirements spec.</t>
+  </si>
+  <si>
+    <t>Final Report: Executive Summary</t>
+  </si>
+  <si>
+    <t>Henry, Robert</t>
+  </si>
+  <si>
+    <t>Final System: Help Page design &amp; implementation</t>
+  </si>
+  <si>
+    <t>Final System: Implementation of Voting System</t>
+  </si>
+  <si>
+    <t>Final System Design</t>
+  </si>
+  <si>
+    <t>Final System Implementation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +200,23 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -179,11 +244,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -224,9 +301,12 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$28</c:f>
+              <c:f>Sheet1!$A$4:$A$39</c:f>
               <c:strCache>
-                <c:ptCount val="25"/>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>Prototyping</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>Prototype Specification</c:v>
                 </c:pt>
@@ -249,7 +329,7 @@
                   <c:v>Interim Report: Background research</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Interim Report:  Requirements spec.</c:v>
+                  <c:v>Interim Report: Requirements spec.</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Interim Report: Initial design</c:v>
@@ -267,27 +347,57 @@
                   <c:v>Interim Report: Time plan</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Final System: Implementation</c:v>
+                  <c:v>Final System</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>Final System Design</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Final System: Template Coding</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Final System: Interface Design</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Final System Implementation</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Final System: Help Page design &amp; implementation</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Final System: Implementation of Voting System</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>Final System: Testing</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>Final Report: Updated designs</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Final Report: Discussion on implementation/testing</c:v>
-                </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="25">
+                  <c:v>Final Report</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Final Report: Executive Summary</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Final Report: Introduction</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Final Report: Condensed existing research</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Final Report: Additional research</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Final Report: Discussion on implementation of software</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>Final Report: Summary of what was achieved</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="32">
                   <c:v>Final Report: Reflective comments</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="33">
                   <c:v>Final Report: Appendix with testing</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="34">
                   <c:v>Final Report: Appendix with minutes</c:v>
                 </c:pt>
               </c:strCache>
@@ -295,10 +405,13 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$28</c:f>
+              <c:f>Sheet1!$B$4:$B$39</c:f>
               <c:numCache>
                 <c:formatCode>d/m/yyyy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>40126</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>40126</c:v>
                 </c:pt>
@@ -339,28 +452,55 @@
                   <c:v>40126</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>40148</c:v>
+                  <c:v>40203</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>40168</c:v>
+                  <c:v>40203</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40203</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>40154</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>40161</c:v>
+                  <c:v>40206</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>40227</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40216</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40245</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40217</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40259</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40217</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>40224</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>40224</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>40168</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>40224</c:v>
+                <c:pt idx="29">
+                  <c:v>40228</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>40206</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>40245</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>40247</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>40252</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>40252</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -382,9 +522,12 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$28</c:f>
+              <c:f>Sheet1!$A$4:$A$39</c:f>
               <c:strCache>
-                <c:ptCount val="25"/>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>Prototyping</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>Prototype Specification</c:v>
                 </c:pt>
@@ -407,7 +550,7 @@
                   <c:v>Interim Report: Background research</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Interim Report:  Requirements spec.</c:v>
+                  <c:v>Interim Report: Requirements spec.</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Interim Report: Initial design</c:v>
@@ -425,27 +568,57 @@
                   <c:v>Interim Report: Time plan</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Final System: Implementation</c:v>
+                  <c:v>Final System</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>Final System Design</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Final System: Template Coding</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Final System: Interface Design</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Final System Implementation</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Final System: Help Page design &amp; implementation</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Final System: Implementation of Voting System</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>Final System: Testing</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>Final Report: Updated designs</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Final Report: Discussion on implementation/testing</c:v>
-                </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="25">
+                  <c:v>Final Report</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Final Report: Executive Summary</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Final Report: Introduction</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Final Report: Condensed existing research</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Final Report: Additional research</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Final Report: Discussion on implementation of software</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>Final Report: Summary of what was achieved</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="32">
                   <c:v>Final Report: Reflective comments</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="33">
                   <c:v>Final Report: Appendix with testing</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="34">
                   <c:v>Final Report: Appendix with minutes</c:v>
                 </c:pt>
               </c:strCache>
@@ -453,10 +626,13 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$28</c:f>
+              <c:f>Sheet1!$C$4:$C$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
@@ -497,52 +673,76 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>74</c:v>
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="20">
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="0">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="31">
                   <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="68859392"/>
-        <c:axId val="68860928"/>
+        <c:axId val="77379840"/>
+        <c:axId val="77389824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="68859392"/>
+        <c:axId val="77379840"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68860928"/>
+        <c:crossAx val="77389824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68860928"/>
+        <c:axId val="77389824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="40126"/>
@@ -564,7 +764,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68859392"/>
+        <c:crossAx val="77379840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -573,7 +773,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -585,13 +785,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>526677</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>168089</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>89647</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>123264</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -899,10 +1099,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -910,108 +1110,110 @@
     <col min="1" max="1" width="66.42578125" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
     <col min="3" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:7" ht="15.75">
+      <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="7">
         <v>40126</v>
       </c>
-      <c r="C2">
-        <v>104</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="C2" s="2">
+        <v>137</v>
+      </c>
+      <c r="D2" s="7">
         <f>B2+C2</f>
-        <v>40230</v>
+        <v>40263</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="D3" s="3"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="3">
+      <c r="A4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="12">
         <v>40126</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3">
-        <f t="shared" ref="D4:D27" si="0">B4+C4</f>
-        <v>40128</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
+      <c r="C4" s="11">
+        <v>12</v>
+      </c>
+      <c r="D4" s="12">
+        <f>B4+C4</f>
+        <v>40138</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3">
+        <v>40126</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ref="D5:D38" si="0">B5+C5</f>
         <v>40128</v>
       </c>
-      <c r="C5">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3">
-        <f t="shared" si="0"/>
-        <v>40135</v>
-      </c>
       <c r="E5" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3">
+        <v>40128</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
         <v>40135</v>
       </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6" s="3">
-        <f t="shared" si="0"/>
-        <v>40138</v>
-      </c>
       <c r="E6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3">
         <v>40135</v>
@@ -1024,92 +1226,95 @@
         <v>40138</v>
       </c>
       <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3">
+        <v>40135</v>
+      </c>
+      <c r="C8">
         <v>3</v>
       </c>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>40138</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="12">
         <v>40126</v>
       </c>
-      <c r="C9">
+      <c r="C10" s="11">
         <v>26</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D10" s="12">
         <f t="shared" si="0"/>
         <v>40152</v>
       </c>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="3">
-        <v>40145</v>
-      </c>
-      <c r="C10">
-        <v>6</v>
-      </c>
-      <c r="D10" s="3">
-        <f t="shared" si="0"/>
-        <v>40151</v>
-      </c>
-      <c r="E10" t="s">
-        <v>4</v>
+      <c r="E10" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B11" s="3">
-        <v>40126</v>
+        <v>40145</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" si="0"/>
-        <v>40131</v>
+        <v>40151</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B12" s="3">
-        <v>40129</v>
+        <v>40126</v>
       </c>
       <c r="C12">
         <v>5</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>40134</v>
+        <v>40131</v>
       </c>
       <c r="E12" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B13" s="3">
         <v>40129</v>
@@ -1122,249 +1327,438 @@
         <v>40134</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B14" s="3">
         <v>40129</v>
       </c>
       <c r="C14">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="0"/>
-        <v>40138</v>
+        <v>40134</v>
       </c>
       <c r="E14" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B15" s="3">
         <v>40129</v>
       </c>
       <c r="C15">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D15" s="3">
         <f t="shared" si="0"/>
-        <v>40141</v>
+        <v>40138</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="3">
-        <v>40138</v>
+        <v>40129</v>
       </c>
       <c r="C16">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" si="0"/>
-        <v>40145</v>
+        <v>40141</v>
       </c>
       <c r="E16" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B17" s="3">
+        <v>40138</v>
+      </c>
+      <c r="C17">
+        <v>7</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="0"/>
+        <v>40145</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="3">
         <v>40126</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>5</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D18" s="3">
         <f t="shared" si="0"/>
         <v>40131</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>2</v>
       </c>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="2"/>
-      <c r="B18" s="3"/>
-      <c r="D18" s="3"/>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="3">
-        <v>40148</v>
-      </c>
-      <c r="C19">
-        <v>87</v>
-      </c>
-      <c r="D19" s="3">
-        <f t="shared" si="0"/>
-        <v>40235</v>
-      </c>
-      <c r="E19" t="s">
-        <v>15</v>
-      </c>
+      <c r="B19" s="3"/>
+      <c r="D19" s="3"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="3">
-        <v>40168</v>
-      </c>
-      <c r="C20">
-        <v>74</v>
-      </c>
-      <c r="D20" s="3">
-        <f t="shared" si="0"/>
-        <v>40242</v>
-      </c>
-      <c r="E20" t="s">
-        <v>5</v>
+      <c r="A20" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="12">
+        <v>40203</v>
+      </c>
+      <c r="C20" s="11">
+        <v>59</v>
+      </c>
+      <c r="D20" s="12">
+        <f>B20+C20</f>
+        <v>40262</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="A21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="7">
+        <v>40203</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="2"/>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="3">
-        <v>40154</v>
-      </c>
-      <c r="C22">
-        <v>28</v>
-      </c>
-      <c r="D22" s="3">
-        <f t="shared" si="0"/>
-        <v>40182</v>
+        <v>38</v>
+      </c>
+      <c r="B22" s="6">
+        <v>40203</v>
+      </c>
+      <c r="C22" s="5">
+        <v>7</v>
+      </c>
+      <c r="D22" s="6">
+        <f>B22+C22</f>
+        <v>40210</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="3">
-        <v>40161</v>
-      </c>
-      <c r="C23">
+        <v>39</v>
+      </c>
+      <c r="B23" s="6">
+        <v>40206</v>
+      </c>
+      <c r="C23" s="5">
         <v>21</v>
       </c>
-      <c r="D23" s="3">
-        <f t="shared" si="0"/>
-        <v>40182</v>
+      <c r="D23" s="6">
+        <f>B23+C23</f>
+        <v>40227</v>
       </c>
       <c r="E23" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="3">
-        <v>40224</v>
-      </c>
-      <c r="C24">
-        <v>21</v>
-      </c>
-      <c r="D24" s="3">
-        <f t="shared" si="0"/>
-        <v>40245</v>
-      </c>
-      <c r="E24" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="1"/>
+    <row r="24" spans="1:7" s="2" customFormat="1">
+      <c r="A24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="3">
-        <v>40224</v>
-      </c>
-      <c r="C25">
-        <v>21</v>
-      </c>
-      <c r="D25" s="3">
-        <f t="shared" si="0"/>
-        <v>40245</v>
+        <v>52</v>
+      </c>
+      <c r="B25" s="6">
+        <v>40227</v>
+      </c>
+      <c r="C25" s="5">
+        <v>32</v>
+      </c>
+      <c r="D25" s="6">
+        <f>B25+C25</f>
+        <v>40259</v>
       </c>
       <c r="E25" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B26" s="3">
-        <v>40168</v>
+        <v>40216</v>
       </c>
       <c r="C26">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="D26" s="3">
         <f t="shared" si="0"/>
-        <v>40242</v>
+        <v>40262</v>
       </c>
       <c r="E26" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="B27" s="3">
+        <v>40245</v>
+      </c>
+      <c r="C27">
+        <v>17</v>
+      </c>
+      <c r="D27" s="3">
+        <f>B27+C27</f>
+        <v>40262</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="B28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="12">
+        <v>40217</v>
+      </c>
+      <c r="C29" s="13">
+        <v>46</v>
+      </c>
+      <c r="D29" s="12">
+        <f>B29+C29</f>
+        <v>40263</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="6">
+        <v>40259</v>
+      </c>
+      <c r="C30" s="9">
+        <v>4</v>
+      </c>
+      <c r="D30" s="6">
+        <f>B30+C30</f>
+        <v>40263</v>
+      </c>
+      <c r="E30" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="3">
+        <v>40217</v>
+      </c>
+      <c r="C31" s="4">
+        <v>7</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="0"/>
         <v>40224</v>
       </c>
-      <c r="C27">
+      <c r="E31" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="3">
+        <v>40224</v>
+      </c>
+      <c r="C32" s="4">
+        <v>7</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="0"/>
+        <v>40231</v>
+      </c>
+      <c r="E32" t="s">
+        <v>32</v>
+      </c>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="3">
+        <v>40228</v>
+      </c>
+      <c r="C33" s="4">
+        <v>10</v>
+      </c>
+      <c r="D33" s="3">
+        <f t="shared" si="0"/>
+        <v>40238</v>
+      </c>
+      <c r="E33" t="s">
+        <v>46</v>
+      </c>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="3">
+        <v>40206</v>
+      </c>
+      <c r="C34">
+        <v>21</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="0"/>
+        <v>40227</v>
+      </c>
+      <c r="E34" t="s">
+        <v>44</v>
+      </c>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="3">
+        <v>40245</v>
+      </c>
+      <c r="C35">
         <v>14</v>
       </c>
-      <c r="D27" s="3">
-        <f t="shared" si="0"/>
-        <v>40238</v>
-      </c>
-      <c r="E27" t="s">
-        <v>3</v>
-      </c>
-      <c r="G27" s="1"/>
+      <c r="D35" s="3">
+        <f t="shared" si="0"/>
+        <v>40259</v>
+      </c>
+      <c r="E35" t="s">
+        <v>32</v>
+      </c>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="3">
+        <v>40247</v>
+      </c>
+      <c r="C36">
+        <v>12</v>
+      </c>
+      <c r="D36" s="3">
+        <f t="shared" si="0"/>
+        <v>40259</v>
+      </c>
+      <c r="E36" t="s">
+        <v>32</v>
+      </c>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="3">
+        <v>40252</v>
+      </c>
+      <c r="C37">
+        <v>7</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="0"/>
+        <v>40259</v>
+      </c>
+      <c r="E37" t="s">
+        <v>42</v>
+      </c>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" s="3">
+        <v>40252</v>
+      </c>
+      <c r="C38">
+        <v>7</v>
+      </c>
+      <c r="D38" s="3">
+        <f t="shared" si="0"/>
+        <v>40259</v>
+      </c>
+      <c r="E38" t="s">
+        <v>43</v>
+      </c>
+      <c r="G38" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Time Plan has been edited to reflect the work we have completed thus far.
</commit_message>
<xml_diff>
--- a/doc/Time-Plan.xlsx
+++ b/doc/Time-Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="72">
   <si>
     <t>Democratic Conferencing Tool</t>
   </si>
@@ -45,18 +45,9 @@
     <t>Group Members</t>
   </si>
   <si>
-    <t>Robert, Kit</t>
-  </si>
-  <si>
     <t>Carl, Kit</t>
   </si>
   <si>
-    <t>Tammie, Robert</t>
-  </si>
-  <si>
-    <t>Robert, Billy</t>
-  </si>
-  <si>
     <t>Prototype Specification</t>
   </si>
   <si>
@@ -87,9 +78,6 @@
     <t>Interim Report: Time plan</t>
   </si>
   <si>
-    <t>Final System: Testing</t>
-  </si>
-  <si>
     <t>Final Report: Summary of what was achieved</t>
   </si>
   <si>
@@ -111,36 +99,12 @@
     <t>Final Report</t>
   </si>
   <si>
-    <t>Billy, Robert, Tammie, Carl</t>
-  </si>
-  <si>
     <t>Billy</t>
   </si>
   <si>
-    <t>Robert, Billy, Henry, Carl, Kit, Tammie</t>
-  </si>
-  <si>
-    <t>Final System</t>
-  </si>
-  <si>
-    <t>Robert, Tammie, Henry, Carl</t>
-  </si>
-  <si>
     <t>Prototyping</t>
   </si>
   <si>
-    <t>Robert, Kit, Tammie, Henry</t>
-  </si>
-  <si>
-    <t>Final System: Template Coding</t>
-  </si>
-  <si>
-    <t>Final System: Interface Design</t>
-  </si>
-  <si>
-    <t>Tammie, Carl</t>
-  </si>
-  <si>
     <t>Final Report: Introduction</t>
   </si>
   <si>
@@ -150,9 +114,6 @@
     <t>Billy, Tammie</t>
   </si>
   <si>
-    <t>Billy, Robert, Henry, Carl</t>
-  </si>
-  <si>
     <t>Final Report: Additional research</t>
   </si>
   <si>
@@ -174,16 +135,103 @@
     <t>Henry, Robert</t>
   </si>
   <si>
-    <t>Final System: Help Page design &amp; implementation</t>
-  </si>
-  <si>
-    <t>Final System: Implementation of Voting System</t>
-  </si>
-  <si>
     <t>Final System Design</t>
   </si>
   <si>
     <t>Final System Implementation</t>
+  </si>
+  <si>
+    <t>Final Report: System Walkthrough with screenshots</t>
+  </si>
+  <si>
+    <t>Kit, Robert</t>
+  </si>
+  <si>
+    <t>Billy, Carl, Kit, Robert, Tammie</t>
+  </si>
+  <si>
+    <t>Billy, Carl, Robert, Tammie</t>
+  </si>
+  <si>
+    <t>Carl, Tammie</t>
+  </si>
+  <si>
+    <t>Henry, Robert, Tammie</t>
+  </si>
+  <si>
+    <t>Billy, Carl, Henry, Kit, Robert, Tammie</t>
+  </si>
+  <si>
+    <t>Henry, Kit, Robert, Tammie</t>
+  </si>
+  <si>
+    <t>Robert, Tammie</t>
+  </si>
+  <si>
+    <t>Billy, Carl, Henry, Robert</t>
+  </si>
+  <si>
+    <t>Final Report: Choose layout and structure the report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final System Design: Write mock-ups for help menu </t>
+  </si>
+  <si>
+    <t>Final System Implementation: Help Page design &amp; implementation</t>
+  </si>
+  <si>
+    <t>Final System Implementation: Testing</t>
+  </si>
+  <si>
+    <t>Final Report: Technical Documentation</t>
+  </si>
+  <si>
+    <t>Final System Implementation: Enabling voting results to display</t>
+  </si>
+  <si>
+    <t>Final System Implementation: Implement confirmation e-mails to be sent upon registering</t>
+  </si>
+  <si>
+    <t>Final System Implementation: Allowing users to vote</t>
+  </si>
+  <si>
+    <t>Final System Implementation: Reset the vote timer when the voting has finished</t>
+  </si>
+  <si>
+    <t>Final System Implementation: Make the Javascript counter work correctly</t>
+  </si>
+  <si>
+    <t>Final System Implementation: Allow the room creator to perform extra actions within the room</t>
+  </si>
+  <si>
+    <t>Final System Design: Translate interface designs into HTML/CSS mock-ups</t>
+  </si>
+  <si>
+    <t>Final System Design: Translate initial paper designs into Photoshop or equivalent image editor</t>
+  </si>
+  <si>
+    <t>Final System Design: Interface designs drawn up on paper</t>
+  </si>
+  <si>
+    <t>Final System Design: Research existing systems with user-friendly designs for inspiration</t>
+  </si>
+  <si>
+    <t>Carl, Henry, Tammie</t>
+  </si>
+  <si>
+    <t>Final System Implementation: Display the results of the voting upon completion</t>
+  </si>
+  <si>
+    <t>Final Report: Detailed Time Plan</t>
+  </si>
+  <si>
+    <t>Billy, Robert, Tammie</t>
+  </si>
+  <si>
+    <t>Interim Report: Introduction</t>
+  </si>
+  <si>
+    <t>Interim Report: Executive Summary</t>
   </si>
 </sst>
 </file>
@@ -216,8 +264,7 @@
     </font>
     <font>
       <b/>
-      <u/>
-      <sz val="11"/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -244,23 +291,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -301,9 +347,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$A$39</c:f>
+              <c:f>Sheet1!$A$4:$A$53</c:f>
               <c:strCache>
-                <c:ptCount val="35"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
                   <c:v>Prototyping</c:v>
                 </c:pt>
@@ -323,92 +369,134 @@
                   <c:v>Interim Report</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Interim Report: Executive Summary</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Interim Report: Introduction</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>Interim Report: The Problem</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>Interim Report: Background research</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>Interim Report: Requirements spec.</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>Interim Report: Initial design</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>Interim Report: Key implementation decisions</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>Interim Report: Initial implementation/prototyping</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>Interim Report: Problems encountered so far</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>Interim Report: Time plan</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>Final System</c:v>
-                </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>Final System Design</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>Final System: Template Coding</c:v>
-                </c:pt>
                 <c:pt idx="19">
-                  <c:v>Final System: Interface Design</c:v>
+                  <c:v>Final System Design: Research existing systems with user-friendly designs for inspiration</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>Final System Design: Interface designs drawn up on paper</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Final System Design: Translate initial paper designs into Photoshop or equivalent image editor</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Final System Design: Translate interface designs into HTML/CSS mock-ups</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Final System Design: Write mock-ups for help menu </c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>Final System Implementation</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>Final System: Help Page design &amp; implementation</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Final System: Implementation of Voting System</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>Final System: Testing</c:v>
-                </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
+                  <c:v>Final System Implementation: Help Page design &amp; implementation</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Final System Implementation: Allowing users to vote</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Final System Implementation: Enabling voting results to display</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Final System Implementation: Make the Javascript counter work correctly</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Final System Implementation: Implement confirmation e-mails to be sent upon registering</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Final System Implementation: Reset the vote timer when the voting has finished</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Final System Implementation: Allow the room creator to perform extra actions within the room</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Final System Implementation: Display the results of the voting upon completion</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Final System Implementation: Testing</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>Final Report</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="37">
+                  <c:v>Final Report: Choose layout and structure the report</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>Final Report: Executive Summary</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="39">
                   <c:v>Final Report: Introduction</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="40">
                   <c:v>Final Report: Condensed existing research</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="41">
                   <c:v>Final Report: Additional research</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="42">
+                  <c:v>Final Report: Technical Documentation</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v>Final Report: Discussion on implementation of software</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="44">
+                  <c:v>Final Report: System Walkthrough with screenshots</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>Final Report: Summary of what was achieved</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="46">
                   <c:v>Final Report: Reflective comments</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="47">
                   <c:v>Final Report: Appendix with testing</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="48">
                   <c:v>Final Report: Appendix with minutes</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>Final Report: Detailed Time Plan</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$39</c:f>
+              <c:f>Sheet1!$B$4:$B$53</c:f>
               <c:numCache>
                 <c:formatCode>d/m/yyyy</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
                   <c:v>40126</c:v>
                 </c:pt>
@@ -434,10 +522,10 @@
                   <c:v>40126</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40129</c:v>
+                  <c:v>40145</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>40129</c:v>
+                  <c:v>40126</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>40129</c:v>
@@ -446,61 +534,106 @@
                   <c:v>40129</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>40129</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40129</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>40138</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>40126</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>40203</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>40203</c:v>
-                </c:pt>
                 <c:pt idx="18">
-                  <c:v>40203</c:v>
+                  <c:v>40210</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>40206</c:v>
+                  <c:v>40210</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40213</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>40220</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40224</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40219</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40219</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>40227</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="27">
                   <c:v>40216</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="28">
+                  <c:v>40227</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>40224</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>40221</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>40214</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>40224</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>40226</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>40245</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="36">
                   <c:v>40217</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="37">
+                  <c:v>40217</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>40259</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="39">
                   <c:v>40217</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="40">
                   <c:v>40224</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="41">
                   <c:v>40228</c:v>
                 </c:pt>
-                <c:pt idx="30">
-                  <c:v>40206</c:v>
-                </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="42">
+                  <c:v>40224</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>40234</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>40238</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>40245</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="46">
                   <c:v>40247</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="47">
                   <c:v>40252</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="48">
                   <c:v>40252</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>40224</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -522,9 +655,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$A$39</c:f>
+              <c:f>Sheet1!$A$4:$A$53</c:f>
               <c:strCache>
-                <c:ptCount val="35"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
                   <c:v>Prototyping</c:v>
                 </c:pt>
@@ -544,92 +677,134 @@
                   <c:v>Interim Report</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Interim Report: Executive Summary</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Interim Report: Introduction</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>Interim Report: The Problem</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>Interim Report: Background research</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>Interim Report: Requirements spec.</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>Interim Report: Initial design</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>Interim Report: Key implementation decisions</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>Interim Report: Initial implementation/prototyping</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>Interim Report: Problems encountered so far</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>Interim Report: Time plan</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>Final System</c:v>
-                </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>Final System Design</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>Final System: Template Coding</c:v>
-                </c:pt>
                 <c:pt idx="19">
-                  <c:v>Final System: Interface Design</c:v>
+                  <c:v>Final System Design: Research existing systems with user-friendly designs for inspiration</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>Final System Design: Interface designs drawn up on paper</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Final System Design: Translate initial paper designs into Photoshop or equivalent image editor</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Final System Design: Translate interface designs into HTML/CSS mock-ups</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Final System Design: Write mock-ups for help menu </c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>Final System Implementation</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>Final System: Help Page design &amp; implementation</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Final System: Implementation of Voting System</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>Final System: Testing</c:v>
-                </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
+                  <c:v>Final System Implementation: Help Page design &amp; implementation</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Final System Implementation: Allowing users to vote</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Final System Implementation: Enabling voting results to display</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Final System Implementation: Make the Javascript counter work correctly</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Final System Implementation: Implement confirmation e-mails to be sent upon registering</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Final System Implementation: Reset the vote timer when the voting has finished</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Final System Implementation: Allow the room creator to perform extra actions within the room</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Final System Implementation: Display the results of the voting upon completion</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Final System Implementation: Testing</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>Final Report</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="37">
+                  <c:v>Final Report: Choose layout and structure the report</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>Final Report: Executive Summary</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="39">
                   <c:v>Final Report: Introduction</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="40">
                   <c:v>Final Report: Condensed existing research</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="41">
                   <c:v>Final Report: Additional research</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="42">
+                  <c:v>Final Report: Technical Documentation</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v>Final Report: Discussion on implementation of software</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="44">
+                  <c:v>Final Report: System Walkthrough with screenshots</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>Final Report: Summary of what was achieved</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="46">
                   <c:v>Final Report: Reflective comments</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="47">
                   <c:v>Final Report: Appendix with testing</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="48">
                   <c:v>Final Report: Appendix with minutes</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>Final Report: Detailed Time Plan</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$C$39</c:f>
+              <c:f>Sheet1!$C$4:$C$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
                   <c:v>12</c:v>
                 </c:pt>
@@ -649,100 +824,148 @@
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>59</c:v>
-                </c:pt>
                 <c:pt idx="18">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>21</c:v>
-                </c:pt>
                 <c:pt idx="21">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="27">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="23">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="25" formatCode="0">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="26" formatCode="0">
+                <c:pt idx="37" formatCode="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="0">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="27" formatCode="0">
+                <c:pt idx="39" formatCode="0">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="28" formatCode="0">
+                <c:pt idx="40" formatCode="0">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="29" formatCode="0">
+                <c:pt idx="41" formatCode="0">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="30">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="42" formatCode="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="32">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>7</c:v>
+                <c:pt idx="44" formatCode="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="77379840"/>
-        <c:axId val="77389824"/>
+        <c:axId val="69117440"/>
+        <c:axId val="69118976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="77379840"/>
+        <c:axId val="69117440"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77389824"/>
+        <c:crossAx val="69118976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77389824"/>
+        <c:axId val="69118976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="40126"/>
@@ -764,7 +987,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77379840"/>
+        <c:crossAx val="69117440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -773,7 +996,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -785,13 +1008,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>526677</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>168089</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>89647</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>123264</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1099,129 +1322,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="66.42578125" customWidth="1"/>
+    <col min="1" max="1" width="88.5703125" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" ht="21">
+      <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" ht="15.75">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="9">
         <v>40126</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="8">
         <v>137</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="9">
         <f>B2+C2</f>
         <v>40263</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>33</v>
+      <c r="E2" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="B3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="12">
+    <row r="4" spans="1:7" ht="15.75">
+      <c r="A4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="9">
         <v>40126</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="8">
         <v>12</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="9">
         <f>B4+C4</f>
         <v>40138</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>37</v>
+      <c r="E4" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="3">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5">
         <v>40126</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>2</v>
       </c>
-      <c r="D5" s="3">
-        <f t="shared" ref="D5:D38" si="0">B5+C5</f>
+      <c r="D5" s="5">
+        <f t="shared" ref="D5:D53" si="0">B5+C5</f>
         <v>40128</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="3">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5">
         <v>40128</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <v>7</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <f t="shared" si="0"/>
         <v>40135</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="3">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5">
         <v>40135</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <v>3</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="5">
         <f t="shared" si="0"/>
         <v>40138</v>
       </c>
@@ -1231,334 +1458,357 @@
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="3">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5">
         <v>40135</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <v>3</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="5">
         <f t="shared" si="0"/>
         <v>40138</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="4"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="12">
+    <row r="10" spans="1:7" ht="15.75">
+      <c r="A10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="9">
         <v>40126</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="8">
         <v>26</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="9">
         <f t="shared" si="0"/>
         <v>40152</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" s="4" customFormat="1">
+      <c r="A11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="5">
+        <v>40145</v>
+      </c>
+      <c r="C11" s="4">
+        <v>7</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="shared" si="0"/>
+        <v>40152</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="12"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="5">
+        <v>40126</v>
+      </c>
+      <c r="C12" s="4">
+        <v>7</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" si="0"/>
+        <v>40133</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="5">
+        <v>40145</v>
+      </c>
+      <c r="C13" s="4">
+        <v>6</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" si="0"/>
+        <v>40151</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="5">
+        <v>40126</v>
+      </c>
+      <c r="C14" s="4">
+        <v>5</v>
+      </c>
+      <c r="D14" s="5">
+        <f t="shared" si="0"/>
+        <v>40131</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="5">
+        <v>40129</v>
+      </c>
+      <c r="C15" s="4">
+        <v>5</v>
+      </c>
+      <c r="D15" s="5">
+        <f t="shared" si="0"/>
+        <v>40134</v>
+      </c>
+      <c r="E15" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="5">
+        <v>40129</v>
+      </c>
+      <c r="C16" s="4">
+        <v>5</v>
+      </c>
+      <c r="D16" s="5">
+        <f t="shared" si="0"/>
+        <v>40134</v>
+      </c>
+      <c r="E16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B17" s="5">
+        <v>40129</v>
+      </c>
+      <c r="C17" s="4">
+        <v>9</v>
+      </c>
+      <c r="D17" s="5">
+        <f t="shared" si="0"/>
+        <v>40138</v>
+      </c>
+      <c r="E17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="5">
+        <v>40129</v>
+      </c>
+      <c r="C18" s="4">
+        <v>12</v>
+      </c>
+      <c r="D18" s="5">
+        <f t="shared" si="0"/>
+        <v>40141</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5">
+        <v>40138</v>
+      </c>
+      <c r="C19" s="4">
+        <v>7</v>
+      </c>
+      <c r="D19" s="5">
+        <f t="shared" si="0"/>
         <v>40145</v>
       </c>
-      <c r="C11">
-        <v>6</v>
-      </c>
-      <c r="D11" s="3">
-        <f t="shared" si="0"/>
-        <v>40151</v>
-      </c>
-      <c r="E11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="3">
+      <c r="E19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5">
         <v>40126</v>
       </c>
-      <c r="C12">
+      <c r="C20" s="4">
         <v>5</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D20" s="5">
         <f t="shared" si="0"/>
         <v>40131</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="4"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75">
+      <c r="A22" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="9">
+        <v>40210</v>
+      </c>
+      <c r="C22" s="8">
+        <v>34</v>
+      </c>
+      <c r="D22" s="9">
+        <f>B22+C22</f>
+        <v>40244</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" s="4" customFormat="1">
+      <c r="A23" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="5">
+        <v>40210</v>
+      </c>
+      <c r="C23" s="4">
         <v>10</v>
       </c>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="3">
-        <v>40129</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="D13" s="3">
-        <f t="shared" si="0"/>
-        <v>40134</v>
-      </c>
-      <c r="E13" t="s">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="3">
-        <v>40129</v>
-      </c>
-      <c r="C14">
-        <v>5</v>
-      </c>
-      <c r="D14" s="3">
-        <f t="shared" si="0"/>
-        <v>40134</v>
-      </c>
-      <c r="E14" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="3">
-        <v>40129</v>
-      </c>
-      <c r="C15">
-        <v>9</v>
-      </c>
-      <c r="D15" s="3">
-        <f t="shared" si="0"/>
-        <v>40138</v>
-      </c>
-      <c r="E15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="3">
-        <v>40129</v>
-      </c>
-      <c r="C16">
-        <v>12</v>
-      </c>
-      <c r="D16" s="3">
-        <f t="shared" si="0"/>
-        <v>40141</v>
-      </c>
-      <c r="E16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="3">
-        <v>40138</v>
-      </c>
-      <c r="C17">
+      <c r="D23" s="5">
+        <f>B23+C23</f>
+        <v>40220</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" s="12"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="5">
+        <v>40213</v>
+      </c>
+      <c r="C24" s="4">
         <v>7</v>
       </c>
-      <c r="D17" s="3">
-        <f t="shared" si="0"/>
-        <v>40145</v>
-      </c>
-      <c r="E17" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="3">
-        <v>40126</v>
-      </c>
-      <c r="C18">
-        <v>5</v>
-      </c>
-      <c r="D18" s="3">
-        <f t="shared" si="0"/>
-        <v>40131</v>
-      </c>
-      <c r="E18" t="s">
-        <v>2</v>
-      </c>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="B19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="12">
-        <v>40203</v>
-      </c>
-      <c r="C20" s="11">
-        <v>59</v>
-      </c>
-      <c r="D20" s="12">
-        <f>B20+C20</f>
-        <v>40262</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="7">
-        <v>40203</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="2"/>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="6">
-        <v>40203</v>
-      </c>
-      <c r="C22" s="5">
-        <v>7</v>
-      </c>
-      <c r="D22" s="6">
-        <f>B22+C22</f>
-        <v>40210</v>
-      </c>
-      <c r="E22" t="s">
-        <v>1</v>
-      </c>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="6">
-        <v>40206</v>
-      </c>
-      <c r="C23" s="5">
-        <v>21</v>
-      </c>
-      <c r="D23" s="6">
-        <f>B23+C23</f>
-        <v>40227</v>
-      </c>
-      <c r="E23" t="s">
-        <v>40</v>
-      </c>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" s="2" customFormat="1">
-      <c r="A24" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="G24" s="10"/>
+      <c r="D24" s="5">
+        <f>B24+C24</f>
+        <v>40220</v>
+      </c>
+      <c r="E24" t="s">
+        <v>45</v>
+      </c>
+      <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="6">
-        <v>40227</v>
-      </c>
-      <c r="C25" s="5">
-        <v>32</v>
-      </c>
-      <c r="D25" s="6">
+        <v>63</v>
+      </c>
+      <c r="B25" s="5">
+        <v>40220</v>
+      </c>
+      <c r="C25" s="4">
+        <v>11</v>
+      </c>
+      <c r="D25" s="5">
         <f>B25+C25</f>
-        <v>40259</v>
+        <v>40231</v>
       </c>
       <c r="E25" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="3">
-        <v>40216</v>
-      </c>
-      <c r="C26">
-        <v>46</v>
-      </c>
-      <c r="D26" s="3">
-        <f t="shared" si="0"/>
-        <v>40262</v>
+        <v>62</v>
+      </c>
+      <c r="B26" s="5">
+        <v>40224</v>
+      </c>
+      <c r="C26" s="4">
+        <v>13</v>
+      </c>
+      <c r="D26" s="5">
+        <f>B26+C26</f>
+        <v>40237</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="3">
-        <v>40245</v>
-      </c>
-      <c r="C27">
-        <v>17</v>
-      </c>
-      <c r="D27" s="3">
+        <v>52</v>
+      </c>
+      <c r="B27" s="5">
+        <v>40219</v>
+      </c>
+      <c r="C27" s="4">
+        <v>7</v>
+      </c>
+      <c r="D27" s="5">
         <f>B27+C27</f>
-        <v>40262</v>
+        <v>40226</v>
       </c>
       <c r="E27" t="s">
         <v>2</v>
@@ -1566,199 +1816,475 @@
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="B28" s="3"/>
-      <c r="D28" s="3"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="4"/>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="12">
-        <v>40217</v>
-      </c>
-      <c r="C29" s="13">
+    <row r="29" spans="1:7" s="2" customFormat="1" ht="15.75">
+      <c r="A29" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="9">
+        <v>40219</v>
+      </c>
+      <c r="C29" s="8">
+        <v>43</v>
+      </c>
+      <c r="D29" s="9">
+        <f>B29+C29</f>
+        <v>40262</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="12">
-        <f>B29+C29</f>
-        <v>40263</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G29" s="1"/>
+      <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" s="6">
+        <v>53</v>
+      </c>
+      <c r="B30" s="5">
+        <v>40227</v>
+      </c>
+      <c r="C30" s="4">
+        <v>32</v>
+      </c>
+      <c r="D30" s="5">
+        <f>B30+C30</f>
         <v>40259</v>
       </c>
-      <c r="C30" s="9">
-        <v>4</v>
-      </c>
-      <c r="D30" s="6">
-        <f>B30+C30</f>
-        <v>40263</v>
-      </c>
       <c r="E30" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" s="3">
-        <v>40217</v>
+        <v>58</v>
+      </c>
+      <c r="B31" s="5">
+        <v>40216</v>
       </c>
       <c r="C31" s="4">
-        <v>7</v>
-      </c>
-      <c r="D31" s="3">
-        <f t="shared" si="0"/>
-        <v>40224</v>
+        <v>14</v>
+      </c>
+      <c r="D31" s="5">
+        <f t="shared" si="0"/>
+        <v>40230</v>
       </c>
       <c r="E31" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32" s="3">
-        <v>40224</v>
+        <v>56</v>
+      </c>
+      <c r="B32" s="5">
+        <v>40227</v>
       </c>
       <c r="C32" s="4">
         <v>7</v>
       </c>
-      <c r="D32" s="3">
-        <f t="shared" si="0"/>
-        <v>40231</v>
+      <c r="D32" s="5">
+        <f t="shared" si="0"/>
+        <v>40234</v>
       </c>
       <c r="E32" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" s="3">
-        <v>40228</v>
+        <v>60</v>
+      </c>
+      <c r="B33" s="5">
+        <v>40224</v>
       </c>
       <c r="C33" s="4">
-        <v>10</v>
-      </c>
-      <c r="D33" s="3">
-        <f t="shared" si="0"/>
-        <v>40238</v>
+        <v>7</v>
+      </c>
+      <c r="D33" s="5">
+        <f t="shared" si="0"/>
+        <v>40231</v>
       </c>
       <c r="E33" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="3">
-        <v>40206</v>
-      </c>
-      <c r="C34">
-        <v>21</v>
-      </c>
-      <c r="D34" s="3">
-        <f t="shared" si="0"/>
-        <v>40227</v>
+        <v>57</v>
+      </c>
+      <c r="B34" s="5">
+        <v>40221</v>
+      </c>
+      <c r="C34" s="4">
+        <v>10</v>
+      </c>
+      <c r="D34" s="5">
+        <f t="shared" si="0"/>
+        <v>40231</v>
       </c>
       <c r="E34" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="3">
-        <v>40245</v>
-      </c>
-      <c r="C35">
-        <v>14</v>
-      </c>
-      <c r="D35" s="3">
-        <f t="shared" si="0"/>
-        <v>40259</v>
+        <v>59</v>
+      </c>
+      <c r="B35" s="5">
+        <v>40214</v>
+      </c>
+      <c r="C35" s="4">
+        <v>6</v>
+      </c>
+      <c r="D35" s="5">
+        <f t="shared" si="0"/>
+        <v>40220</v>
       </c>
       <c r="E35" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="3">
-        <v>40247</v>
-      </c>
-      <c r="C36">
-        <v>12</v>
-      </c>
-      <c r="D36" s="3">
-        <f t="shared" si="0"/>
-        <v>40259</v>
+        <v>61</v>
+      </c>
+      <c r="B36" s="5">
+        <v>40224</v>
+      </c>
+      <c r="C36" s="4">
+        <v>10</v>
+      </c>
+      <c r="D36" s="5">
+        <f t="shared" si="0"/>
+        <v>40234</v>
       </c>
       <c r="E36" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="3">
-        <v>40252</v>
-      </c>
-      <c r="C37">
-        <v>7</v>
-      </c>
-      <c r="D37" s="3">
-        <f t="shared" si="0"/>
-        <v>40259</v>
+        <v>67</v>
+      </c>
+      <c r="B37" s="5">
+        <v>40226</v>
+      </c>
+      <c r="C37" s="4">
+        <v>8</v>
+      </c>
+      <c r="D37" s="5">
+        <f t="shared" si="0"/>
+        <v>40234</v>
       </c>
       <c r="E37" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>28</v>
-      </c>
-      <c r="B38" s="3">
+        <v>54</v>
+      </c>
+      <c r="B38" s="5">
+        <v>40245</v>
+      </c>
+      <c r="C38" s="4">
+        <v>17</v>
+      </c>
+      <c r="D38" s="5">
+        <f>B38+C38</f>
+        <v>40262</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="4"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="4"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" ht="15.75">
+      <c r="A40" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="9">
+        <v>40217</v>
+      </c>
+      <c r="C40" s="11">
+        <v>46</v>
+      </c>
+      <c r="D40" s="9">
+        <f>B40+C40</f>
+        <v>40263</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" s="4" customFormat="1">
+      <c r="A41" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" s="5">
+        <v>40217</v>
+      </c>
+      <c r="C41" s="6">
+        <v>3</v>
+      </c>
+      <c r="D41" s="5">
+        <f>B41+C41</f>
+        <v>40220</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G41" s="12"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="5">
+        <v>40259</v>
+      </c>
+      <c r="C42" s="6">
+        <v>4</v>
+      </c>
+      <c r="D42" s="5">
+        <f>B42+C42</f>
+        <v>40263</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" s="5">
+        <v>40217</v>
+      </c>
+      <c r="C43" s="6">
+        <v>7</v>
+      </c>
+      <c r="D43" s="5">
+        <f t="shared" si="0"/>
+        <v>40224</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" s="5">
+        <v>40224</v>
+      </c>
+      <c r="C44" s="6">
+        <v>7</v>
+      </c>
+      <c r="D44" s="5">
+        <f t="shared" si="0"/>
+        <v>40231</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" s="5">
+        <v>40228</v>
+      </c>
+      <c r="C45" s="6">
+        <v>10</v>
+      </c>
+      <c r="D45" s="5">
+        <f t="shared" si="0"/>
+        <v>40238</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" s="5">
+        <v>40224</v>
+      </c>
+      <c r="C46" s="6">
+        <v>10</v>
+      </c>
+      <c r="D46" s="5">
+        <f t="shared" si="0"/>
+        <v>40234</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" s="5">
+        <v>40234</v>
+      </c>
+      <c r="C47" s="4">
+        <v>14</v>
+      </c>
+      <c r="D47" s="5">
+        <f t="shared" si="0"/>
+        <v>40248</v>
+      </c>
+      <c r="E47" t="s">
+        <v>50</v>
+      </c>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" s="5">
+        <v>40238</v>
+      </c>
+      <c r="C48" s="6">
+        <v>24</v>
+      </c>
+      <c r="D48" s="5">
+        <f t="shared" si="0"/>
+        <v>40262</v>
+      </c>
+      <c r="E48" t="s">
+        <v>31</v>
+      </c>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" s="5">
+        <v>40245</v>
+      </c>
+      <c r="C49" s="4">
+        <v>14</v>
+      </c>
+      <c r="D49" s="5">
+        <f t="shared" si="0"/>
+        <v>40259</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" s="5">
+        <v>40247</v>
+      </c>
+      <c r="C50" s="4">
+        <v>14</v>
+      </c>
+      <c r="D50" s="5">
+        <f t="shared" si="0"/>
+        <v>40261</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="5">
         <v>40252</v>
       </c>
-      <c r="C38">
-        <v>7</v>
-      </c>
-      <c r="D38" s="3">
-        <f t="shared" si="0"/>
-        <v>40259</v>
-      </c>
-      <c r="E38" t="s">
-        <v>43</v>
-      </c>
-      <c r="G38" s="1"/>
+      <c r="C51" s="4">
+        <v>10</v>
+      </c>
+      <c r="D51" s="5">
+        <f t="shared" si="0"/>
+        <v>40262</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B52" s="5">
+        <v>40252</v>
+      </c>
+      <c r="C52" s="4">
+        <v>10</v>
+      </c>
+      <c r="D52" s="5">
+        <f t="shared" si="0"/>
+        <v>40262</v>
+      </c>
+      <c r="E52" t="s">
+        <v>31</v>
+      </c>
+      <c r="G52" s="1"/>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B53" s="3">
+        <v>40224</v>
+      </c>
+      <c r="C53" s="4">
+        <v>10</v>
+      </c>
+      <c r="D53" s="5">
+        <f t="shared" si="0"/>
+        <v>40234</v>
+      </c>
+      <c r="E53" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Quick edit to the Time Plan and Final Report.  Unable to proceed with the report writing until further progress made.  Discuss tomorrow.
</commit_message>
<xml_diff>
--- a/doc/Time-Plan.xlsx
+++ b/doc/Time-Plan.xlsx
@@ -948,24 +948,24 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="69117440"/>
-        <c:axId val="69118976"/>
+        <c:axId val="76330496"/>
+        <c:axId val="76332032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="69117440"/>
+        <c:axId val="76330496"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69118976"/>
+        <c:crossAx val="76332032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69118976"/>
+        <c:axId val="76332032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="40126"/>
@@ -987,7 +987,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69117440"/>
+        <c:crossAx val="76330496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -996,7 +996,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1325,7 +1325,7 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1712,7 +1712,7 @@
         <v>34</v>
       </c>
       <c r="D22" s="9">
-        <f>B22+C22</f>
+        <f t="shared" ref="D22:D27" si="1">B22+C22</f>
         <v>40244</v>
       </c>
       <c r="E22" s="8" t="s">
@@ -1731,7 +1731,7 @@
         <v>10</v>
       </c>
       <c r="D23" s="5">
-        <f>B23+C23</f>
+        <f t="shared" si="1"/>
         <v>40220</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -1750,7 +1750,7 @@
         <v>7</v>
       </c>
       <c r="D24" s="5">
-        <f>B24+C24</f>
+        <f t="shared" si="1"/>
         <v>40220</v>
       </c>
       <c r="E24" t="s">
@@ -1769,7 +1769,7 @@
         <v>11</v>
       </c>
       <c r="D25" s="5">
-        <f>B25+C25</f>
+        <f t="shared" si="1"/>
         <v>40231</v>
       </c>
       <c r="E25" t="s">
@@ -1788,7 +1788,7 @@
         <v>13</v>
       </c>
       <c r="D26" s="5">
-        <f>B26+C26</f>
+        <f t="shared" si="1"/>
         <v>40237</v>
       </c>
       <c r="E26" t="s">
@@ -1807,7 +1807,7 @@
         <v>7</v>
       </c>
       <c r="D27" s="5">
-        <f>B27+C27</f>
+        <f t="shared" si="1"/>
         <v>40226</v>
       </c>
       <c r="E27" t="s">

</xml_diff>

<commit_message>
Added more to the Time Plan to reflect current to-do list.
</commit_message>
<xml_diff>
--- a/doc/Time-Plan.xlsx
+++ b/doc/Time-Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="54">
   <si>
     <t>Robert</t>
   </si>
@@ -165,7 +165,19 @@
     <t>x</t>
   </si>
   <si>
-    <t>/</t>
+    <t xml:space="preserve"> -</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Final System Implementation: Commenting of all source code</t>
+  </si>
+  <si>
+    <t>Final System Implementation: Detailed system messages to be displayed</t>
+  </si>
+  <si>
+    <t>Final System Design: Project logo design</t>
   </si>
 </sst>
 </file>
@@ -209,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -232,6 +244,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -274,9 +292,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$31</c:f>
+              <c:f>Sheet1!$A$3:$A$34</c:f>
               <c:strCache>
-                <c:ptCount val="29"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>Final System Design</c:v>
                 </c:pt>
@@ -295,67 +313,76 @@
                 <c:pt idx="5">
                   <c:v>Final System Design: Translate interface designs into HTML/CSS mock-ups</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="6">
+                  <c:v>Final System Design: Project logo design</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Final System Implementation</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Final System Implementation: Help Page design &amp; implementation</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Final System Implementation: Allowing users to vote</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>Final System Implementation: Enabling voting results to display</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>Final System Implementation: Make the Javascript counter work correctly</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>Final System Implementation: Implement confirmation e-mails to be sent upon registering</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>Final System Implementation: Reset the vote timer when the voting has finished</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Final System Implementation: Allow the room creator to perform extra actions within the room</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>Final System Implementation: Display the results of the voting upon completion</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
+                  <c:v>Final System Implementation: Commenting of all source code</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Final System Implementation: Detailed system messages to be displayed</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Final System Implementation: Testing</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>Final Report</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>Final Report: Choose layout and structure the report</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>Final Report: Introduction</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="24">
                   <c:v>Final Report: Condensed existing research</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="25">
                   <c:v>Final Report: Discussion on implementation of software</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
                   <c:v>Final Report: Detailed Time Plan</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="27">
                   <c:v>Final Report: System Walkthrough with screenshots</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="28">
                   <c:v>Final Report: Summary of what was achieved</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="29">
                   <c:v>Final Report: Reflective comments</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="30">
                   <c:v>Final Report: Appendix with testing</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="31">
                   <c:v>Final Report: Appendix with minutes</c:v>
                 </c:pt>
               </c:strCache>
@@ -363,10 +390,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$31</c:f>
+              <c:f>Sheet1!$B$3:$B$34</c:f>
               <c:numCache>
                 <c:formatCode>d/m/yyyy</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>40210</c:v>
                 </c:pt>
@@ -385,67 +412,76 @@
                 <c:pt idx="5">
                   <c:v>40237</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="6">
+                  <c:v>40238</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>40219</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>40227</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>40216</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>40227</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>40224</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>40221</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>40214</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>40224</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>40226</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
+                  <c:v>40244</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40244</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>40245</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>40217</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>40217</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>40217</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="24">
                   <c:v>40224</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="25">
                   <c:v>40234</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
                   <c:v>40224</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="27">
                   <c:v>40238</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="28">
                   <c:v>40245</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="29">
                   <c:v>40247</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="30">
                   <c:v>40252</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="31">
                   <c:v>40252</c:v>
                 </c:pt>
               </c:numCache>
@@ -468,9 +504,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$31</c:f>
+              <c:f>Sheet1!$A$3:$A$34</c:f>
               <c:strCache>
-                <c:ptCount val="29"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>Final System Design</c:v>
                 </c:pt>
@@ -489,67 +525,76 @@
                 <c:pt idx="5">
                   <c:v>Final System Design: Translate interface designs into HTML/CSS mock-ups</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="6">
+                  <c:v>Final System Design: Project logo design</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Final System Implementation</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Final System Implementation: Help Page design &amp; implementation</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Final System Implementation: Allowing users to vote</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>Final System Implementation: Enabling voting results to display</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>Final System Implementation: Make the Javascript counter work correctly</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>Final System Implementation: Implement confirmation e-mails to be sent upon registering</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>Final System Implementation: Reset the vote timer when the voting has finished</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Final System Implementation: Allow the room creator to perform extra actions within the room</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>Final System Implementation: Display the results of the voting upon completion</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
+                  <c:v>Final System Implementation: Commenting of all source code</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Final System Implementation: Detailed system messages to be displayed</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Final System Implementation: Testing</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>Final Report</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>Final Report: Choose layout and structure the report</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>Final Report: Introduction</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="24">
                   <c:v>Final Report: Condensed existing research</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="25">
                   <c:v>Final Report: Discussion on implementation of software</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
                   <c:v>Final Report: Detailed Time Plan</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="27">
                   <c:v>Final Report: System Walkthrough with screenshots</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="28">
                   <c:v>Final Report: Summary of what was achieved</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="29">
                   <c:v>Final Report: Reflective comments</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="30">
                   <c:v>Final Report: Appendix with testing</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="31">
                   <c:v>Final Report: Appendix with minutes</c:v>
                 </c:pt>
               </c:strCache>
@@ -557,10 +602,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$31</c:f>
+              <c:f>Sheet1!$C$3:$C$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>41</c:v>
                 </c:pt>
@@ -579,67 +624,76 @@
                 <c:pt idx="5">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="0">
+                <c:pt idx="21" formatCode="0">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="0">
+                <c:pt idx="22" formatCode="0">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="0">
+                <c:pt idx="23" formatCode="0">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="21" formatCode="0">
+                <c:pt idx="24" formatCode="0">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="25">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="24" formatCode="0">
+                <c:pt idx="27" formatCode="0">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="28">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="29">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="30">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="31">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -647,11 +701,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="75097600"/>
-        <c:axId val="75099136"/>
+        <c:axId val="68921600"/>
+        <c:axId val="69271552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="75097600"/>
+        <c:axId val="68921600"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -667,14 +721,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75099136"/>
+        <c:crossAx val="69271552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75099136"/>
+        <c:axId val="69271552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="40268"/>
@@ -697,7 +751,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75097600"/>
+        <c:crossAx val="68921600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -706,7 +760,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -718,14 +772,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>414619</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>33619</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>56029</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>324971</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>179295</xdr:rowOff>
+      <xdr:rowOff>100854</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1032,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1045,7 +1099,7 @@
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="34.42578125" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1063,6 +1117,9 @@
       </c>
       <c r="E1" s="6" t="s">
         <v>6</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1089,6 +1146,7 @@
       <c r="E3" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="F3" s="12"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" s="3" customFormat="1">
@@ -1108,7 +1166,7 @@
       <c r="E4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="12" t="s">
         <v>48</v>
       </c>
       <c r="G4" s="5"/>
@@ -1130,7 +1188,7 @@
       <c r="E5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="12" t="s">
         <v>48</v>
       </c>
       <c r="G5" s="1"/>
@@ -1152,7 +1210,7 @@
       <c r="E6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="12" t="s">
         <v>48</v>
       </c>
       <c r="G6" s="1"/>
@@ -1174,7 +1232,7 @@
       <c r="E7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="12" t="s">
         <v>49</v>
       </c>
       <c r="G7" s="1"/>
@@ -1196,135 +1254,137 @@
       <c r="E8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="12" t="s">
         <v>49</v>
       </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="3"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="3"/>
+      <c r="A9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="8">
+        <v>40238</v>
+      </c>
+      <c r="C9" s="9">
+        <v>20</v>
+      </c>
+      <c r="D9" s="8">
+        <f>B9+C9</f>
+        <v>40258</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>49</v>
+      </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" s="2" customFormat="1">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:7">
+      <c r="A10" s="3"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" s="2" customFormat="1">
+      <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B11" s="7">
         <v>40219</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C11" s="6">
         <v>43</v>
       </c>
-      <c r="D10" s="7">
-        <f>B10+C10</f>
+      <c r="D11" s="7">
+        <f>B11+C11</f>
         <v>40262</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="8">
-        <v>40227</v>
-      </c>
-      <c r="C11" s="9">
-        <v>32</v>
-      </c>
-      <c r="D11" s="8">
-        <f>B11+C11</f>
-        <v>40259</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="1"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B12" s="8">
-        <v>40216</v>
+        <v>40227</v>
       </c>
       <c r="C12" s="9">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="D12" s="8">
-        <f t="shared" ref="D12:D31" si="1">B12+C12</f>
-        <v>40230</v>
+        <f>B12+C12</f>
+        <v>40259</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="12" t="s">
         <v>48</v>
       </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="8">
+        <v>40216</v>
+      </c>
+      <c r="C13" s="9">
+        <v>14</v>
+      </c>
+      <c r="D13" s="8">
+        <f t="shared" ref="D13:D34" si="1">B13+C13</f>
+        <v>40230</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B14" s="8">
         <v>40227</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C14" s="9">
         <v>7</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D14" s="8">
         <f t="shared" si="1"/>
         <v>40234</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F13" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="8">
-        <v>40224</v>
-      </c>
-      <c r="C14" s="9">
-        <v>7</v>
-      </c>
-      <c r="D14" s="8">
-        <f t="shared" si="1"/>
-        <v>40231</v>
-      </c>
       <c r="E14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="12" t="s">
         <v>48</v>
       </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B15" s="8">
-        <v>40221</v>
+        <v>40224</v>
       </c>
       <c r="C15" s="9">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D15" s="8">
         <f t="shared" si="1"/>
@@ -1333,64 +1393,64 @@
       <c r="E15" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="12" t="s">
         <v>48</v>
       </c>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B16" s="8">
-        <v>40214</v>
+        <v>40221</v>
       </c>
       <c r="C16" s="9">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D16" s="8">
         <f t="shared" si="1"/>
-        <v>40220</v>
+        <v>40231</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="12" t="s">
         <v>48</v>
       </c>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" s="8">
-        <v>40224</v>
+        <v>40214</v>
       </c>
       <c r="C17" s="9">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D17" s="8">
         <f t="shared" si="1"/>
-        <v>40234</v>
+        <v>40220</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="12" t="s">
         <v>48</v>
       </c>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B18" s="8">
-        <v>40226</v>
+        <v>40224</v>
       </c>
       <c r="C18" s="9">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D18" s="8">
         <f t="shared" si="1"/>
@@ -1399,344 +1459,412 @@
       <c r="E18" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="12" t="s">
         <v>48</v>
       </c>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="8">
+        <v>40226</v>
+      </c>
+      <c r="C19" s="9">
+        <v>8</v>
+      </c>
+      <c r="D19" s="8">
+        <f t="shared" si="1"/>
+        <v>40234</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="8">
+        <v>40244</v>
+      </c>
+      <c r="C20" s="9">
+        <v>7</v>
+      </c>
+      <c r="D20" s="8">
+        <f t="shared" si="1"/>
+        <v>40251</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="8">
+        <v>40244</v>
+      </c>
+      <c r="C21" s="9">
+        <v>7</v>
+      </c>
+      <c r="D21" s="8">
+        <f t="shared" si="1"/>
+        <v>40251</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B22" s="8">
         <v>40245</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C22" s="9">
         <v>17</v>
-      </c>
-      <c r="D19" s="8">
-        <f>B19+C19</f>
-        <v>40262</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="3"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="3"/>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="7">
-        <v>40217</v>
-      </c>
-      <c r="C21" s="10">
-        <v>46</v>
-      </c>
-      <c r="D21" s="7">
-        <f>B21+C21</f>
-        <v>40263</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" s="3" customFormat="1">
-      <c r="A22" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="8">
-        <v>40217</v>
-      </c>
-      <c r="C22" s="11">
-        <v>3</v>
       </c>
       <c r="D22" s="8">
         <f>B22+C22</f>
+        <v>40262</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="3"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="7">
+        <v>40217</v>
+      </c>
+      <c r="C24" s="10">
+        <v>46</v>
+      </c>
+      <c r="D24" s="7">
+        <f>B24+C24</f>
+        <v>40263</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" s="3" customFormat="1">
+      <c r="A25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="8">
+        <v>40217</v>
+      </c>
+      <c r="C25" s="11">
+        <v>3</v>
+      </c>
+      <c r="D25" s="8">
+        <f>B25+C25</f>
         <v>40220</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F25" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="3" t="s">
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B26" s="8">
         <v>40217</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C26" s="11">
         <v>7</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D26" s="8">
         <f t="shared" si="1"/>
         <v>40224</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F26" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="3" t="s">
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B27" s="8">
         <v>40224</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C27" s="11">
         <v>7</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D27" s="8">
         <f t="shared" si="1"/>
         <v>40231</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F27" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="3" t="s">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B28" s="8">
         <v>40234</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C28" s="9">
         <v>7</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D28" s="8">
         <f t="shared" si="1"/>
         <v>40241</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F28" s="12" t="s">
         <v>48</v>
-      </c>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="8">
-        <v>40224</v>
-      </c>
-      <c r="C26" s="9">
-        <v>10</v>
-      </c>
-      <c r="D26" s="8">
-        <f>B26+C26</f>
-        <v>40234</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="8">
-        <v>40238</v>
-      </c>
-      <c r="C27" s="11">
-        <v>24</v>
-      </c>
-      <c r="D27" s="8">
-        <f t="shared" si="1"/>
-        <v>40262</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" t="s">
-        <v>49</v>
-      </c>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="8">
-        <v>40245</v>
-      </c>
-      <c r="C28" s="9">
-        <v>14</v>
-      </c>
-      <c r="D28" s="8">
-        <f t="shared" si="1"/>
-        <v>40259</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" t="s">
-        <v>49</v>
       </c>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="3" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="B29" s="8">
-        <v>40247</v>
+        <v>40224</v>
       </c>
       <c r="C29" s="9">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D29" s="8">
-        <f t="shared" si="1"/>
-        <v>40261</v>
+        <f>B29+C29</f>
+        <v>40234</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F29" t="s">
-        <v>49</v>
-      </c>
-      <c r="G29" s="1"/>
+      <c r="F29" s="12" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="3" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B30" s="8">
-        <v>40252</v>
-      </c>
-      <c r="C30" s="9">
-        <v>10</v>
+        <v>40238</v>
+      </c>
+      <c r="C30" s="11">
+        <v>24</v>
       </c>
       <c r="D30" s="8">
         <f t="shared" si="1"/>
         <v>40262</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="12" t="s">
         <v>49</v>
       </c>
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B31" s="8">
-        <v>40252</v>
+        <v>40245</v>
       </c>
       <c r="C31" s="9">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D31" s="8">
         <f t="shared" si="1"/>
-        <v>40262</v>
+        <v>40259</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="12" t="s">
         <v>49</v>
       </c>
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B32" s="8">
-        <v>40237</v>
-      </c>
-      <c r="C32" s="11">
+        <v>40247</v>
+      </c>
+      <c r="C32" s="9">
         <v>14</v>
       </c>
       <c r="D32" s="8">
-        <f>B32+C32</f>
-        <v>40251</v>
+        <f t="shared" si="1"/>
+        <v>40261</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="12" t="s">
         <v>49</v>
       </c>
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" t="s">
-        <v>34</v>
+      <c r="A33" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B33" s="8">
-        <v>40224</v>
-      </c>
-      <c r="C33" s="11">
+        <v>40252</v>
+      </c>
+      <c r="C33" s="9">
         <v>10</v>
       </c>
       <c r="D33" s="8">
-        <f>B33+C33</f>
-        <v>40234</v>
+        <f t="shared" si="1"/>
+        <v>40262</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="12" t="s">
         <v>49</v>
       </c>
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="8">
+        <v>40252</v>
+      </c>
+      <c r="C34" s="9">
+        <v>10</v>
+      </c>
+      <c r="D34" s="8">
+        <f t="shared" si="1"/>
+        <v>40262</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="8">
+        <v>40237</v>
+      </c>
+      <c r="C35" s="11">
+        <v>14</v>
+      </c>
+      <c r="D35" s="8">
+        <f>B35+C35</f>
+        <v>40251</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="8">
+        <v>40224</v>
+      </c>
+      <c r="C36" s="11">
+        <v>10</v>
+      </c>
+      <c r="D36" s="8">
+        <f>B36+C36</f>
+        <v>40234</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B37" s="8">
         <v>40259</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C37" s="11">
         <v>4</v>
       </c>
-      <c r="D34" s="8">
-        <f>B34+C34</f>
+      <c r="D37" s="8">
+        <f>B37+C37</f>
         <v>40263</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F37" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="G34" s="1"/>
+      <c r="G37" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes to the Final Report - Added to research section
</commit_message>
<xml_diff>
--- a/doc/Time-Plan.xlsx
+++ b/doc/Time-Plan.xlsx
@@ -266,7 +266,17 @@
   <c:lang val="en-GB"/>
   <c:chart>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.34073200820611382"/>
+          <c:y val="8.1104721063573984E-2"/>
+          <c:w val="0.61073775575815681"/>
+          <c:h val="0.88982531953696653"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="stacked"/>
@@ -701,11 +711,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="68921600"/>
-        <c:axId val="69271552"/>
+        <c:axId val="77375744"/>
+        <c:axId val="77725696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="68921600"/>
+        <c:axId val="77375744"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -721,14 +731,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69271552"/>
+        <c:crossAx val="77725696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69271552"/>
+        <c:axId val="77725696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="40268"/>
@@ -751,7 +761,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68921600"/>
+        <c:crossAx val="77375744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -760,7 +770,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -771,15 +781,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>414619</xdr:colOff>
+      <xdr:colOff>425825</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>56029</xdr:rowOff>
+      <xdr:rowOff>100853</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>324971</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>100854</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>481853</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>168088</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1088,8 +1098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Changes to the UI documentation within the final report.
</commit_message>
<xml_diff>
--- a/doc/Time-Plan.xlsx
+++ b/doc/Time-Plan.xlsx
@@ -271,8 +271,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.34073200820611382"/>
-          <c:y val="8.1104721063573984E-2"/>
+          <c:x val="0.34073200820611371"/>
+          <c:y val="8.1104721063573998E-2"/>
           <c:w val="0.61073775575815681"/>
           <c:h val="0.88982531953696653"/>
         </c:manualLayout>
@@ -711,11 +711,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="77375744"/>
-        <c:axId val="77725696"/>
+        <c:axId val="68921600"/>
+        <c:axId val="69337088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="77375744"/>
+        <c:axId val="68921600"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -731,14 +731,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77725696"/>
+        <c:crossAx val="69337088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77725696"/>
+        <c:axId val="69337088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="40268"/>
@@ -761,7 +761,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77375744"/>
+        <c:crossAx val="68921600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -770,7 +770,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1098,8 +1098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>